<commit_message>
new countdown and other s
</commit_message>
<xml_diff>
--- a/Classifiche.xlsx
+++ b/Classifiche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzoparenti/Desktop/Gran Turismo™ 7/github/worldtourbyTLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1344AFAF-4B4F-0E44-88A0-E6BFBFD2AC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ED17CF-CE8E-5340-B796-91B7E64FD451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="500" windowWidth="27500" windowHeight="16940" activeTab="4" xr2:uid="{0ECEFD28-5025-934F-A4E5-815ACDF49090}"/>
   </bookViews>
@@ -16906,7 +16906,7 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>